<commit_message>
Update Scenario Key scenario descriptions
</commit_message>
<xml_diff>
--- a/DoArtOutputs/Scenario_Key.xlsx
+++ b/DoArtOutputs/Scenario_Key.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20366"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20375"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\HHCoM\DoArtOutputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5601424A-9739-4E5C-8154-A7C3C1C4013B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2BCDB8-A7C7-4786-B6CF-4EFE8F283FCD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8150" xr2:uid="{B2D28D4D-ABA9-44E8-9BE6-F5182B7E3B2C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{B2D28D4D-ABA9-44E8-9BE6-F5182B7E3B2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,45 +36,15 @@
     <t>2a</t>
   </si>
   <si>
-    <t>Females</t>
-  </si>
-  <si>
-    <t>Males</t>
-  </si>
-  <si>
     <t>Sex</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Clinic ART only</t>
-  </si>
-  <si>
-    <t>Clinic ART + Additional HTC campaign every 5 years + Community-based ART for people not reached by standard of care</t>
-  </si>
-  <si>
-    <t>Clinic ART + Additional HTC campaign every 5 years</t>
-  </si>
-  <si>
     <t>Percent virally suppressed</t>
   </si>
   <si>
-    <t>88.9% * 70% = 62.23% (HSRC, DO ART)​</t>
-  </si>
-  <si>
-    <t>78% * 51% = 39.78% (HSRC, DO ART)</t>
-  </si>
-  <si>
-    <t>90% * 73% = 65.7%​ (DO ART)</t>
-  </si>
-  <si>
-    <t>91% * 72% = 65.5%​ (DO ART)</t>
-  </si>
-  <si>
-    <t>95-95-95</t>
-  </si>
-  <si>
     <t>85.7% (assumed)</t>
   </si>
   <si>
@@ -84,10 +54,40 @@
     <t>VMMC additionally scaled up to 72% across all age groups by 2030</t>
   </si>
   <si>
-    <t>91% * 51% = 46.41% (DO ART)</t>
-  </si>
-  <si>
-    <t>90% * 70% = 63.00% (DO ART)</t>
+    <t>Baseline HIV testing + Clinic ART only</t>
+  </si>
+  <si>
+    <t>Baseline HIV testing + Clinic ART + Additional Home HTC campaigns once every 5 years + Community-based ART for people not reached by standard of care</t>
+  </si>
+  <si>
+    <t>Baseline HIV testing + Clinic ART + Additional Home HTC campaigns once every 5 years</t>
+  </si>
+  <si>
+    <t>UNAIDS 95-95-95 target</t>
+  </si>
+  <si>
+    <t>Women</t>
+  </si>
+  <si>
+    <t>Men</t>
+  </si>
+  <si>
+    <t>88.9% * 70% = 62.23% (SABSSMV, DO ART)​</t>
+  </si>
+  <si>
+    <t>78% * 51% = 39.78% (SABSSMV, DO ART)</t>
+  </si>
+  <si>
+    <t>~93% (75% x (100% - 88.9%) HTC 1x/5 years ) * 73% = ~68%​ (SABSSMV, Sharma, DO ART)</t>
+  </si>
+  <si>
+    <t>~93% (75% x (100% - 88.9%) HTC 1x/5 years ) * 70% = ~65% (SABSSMV, Sharma, DO ART)</t>
+  </si>
+  <si>
+    <t>~92% (75% x (100% - 78%) HTC 1x/5 years) * 72% = ~66%​ (SABSSMV, Sharma, DO ART)</t>
+  </si>
+  <si>
+    <t>~92% (75% x (100% - 78%) HTC 1x/5 years) * 51% = ~47% (SABSSMV, Sharma, DO ART)</t>
   </si>
 </sst>
 </file>
@@ -146,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -163,6 +163,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -481,18 +484,18 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.1796875" customWidth="1"/>
-    <col min="5" max="5" width="32.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
+    <col min="5" max="5" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -500,51 +503,51 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>7</v>
+      <c r="C2" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="C3" s="6"/>
       <c r="D3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -552,29 +555,29 @@
         <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="E4" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
       <c r="D5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="E5" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
@@ -582,29 +585,29 @@
         <v>4</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>20</v>
+        <v>13</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
       <c r="D7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>3</v>
       </c>
@@ -612,29 +615,29 @@
         <v>3</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="3" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>

</xml_diff>